<commit_message>
sn: update itas forms
</commit_message>
<xml_diff>
--- a/LF/ITAS/sn_lf_itas_20305_2_fts.xlsx
+++ b/LF/ITAS/sn_lf_itas_20305_2_fts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\LF\ITAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27DA75A6-EB3B-4B48-8F2C-2CA52F8088DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1950561C-0D56-45B2-A038-A1E2B666E1E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="160">
   <si>
     <t>type</t>
   </si>
@@ -483,15 +483,6 @@
     <t>21. Notes supplémentaires</t>
   </si>
   <si>
-    <t>(2024 Mai) 2. ITAS - Formulaire Résultat FTS V3</t>
-  </si>
-  <si>
-    <t>sn_lf_itas_20305_2_fts_v3</t>
-  </si>
-  <si>
-    <t>sn_lf_f_2405_v3</t>
-  </si>
-  <si>
     <t>Absence.de.ligne.temoin/controle</t>
   </si>
   <si>
@@ -514,6 +505,21 @@
   </si>
   <si>
     <t>Insuffisance du volume de sang dû à la pipette</t>
+  </si>
+  <si>
+    <t>Le format du QR Code est incorrect. Exemple SENITAS1234</t>
+  </si>
+  <si>
+    <t>if(${d_eu_name} = 'SARAYA', regex(., '^(SENITAS)\d{4}$'), true())</t>
+  </si>
+  <si>
+    <t>sn_lf_f_2405_v4</t>
+  </si>
+  <si>
+    <t>(2024 Mai) 2. ITAS - Formulaire Résultat FTS V4</t>
+  </si>
+  <si>
+    <t>sn_lf_itas_20305_2_fts_v4</t>
   </si>
 </sst>
 </file>
@@ -1351,7 +1357,7 @@
         <v>96</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="C9" s="37" t="s">
         <v>116</v>
@@ -1459,7 +1465,7 @@
       <c r="L13" s="13"/>
       <c r="M13" s="12"/>
     </row>
-    <row r="14" spans="1:15" s="10" customFormat="1">
+    <row r="14" spans="1:15" s="10" customFormat="1" ht="51">
       <c r="A14" s="12" t="s">
         <v>20</v>
       </c>
@@ -1471,8 +1477,12 @@
       </c>
       <c r="D14" s="15"/>
       <c r="E14" s="13"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="15"/>
+      <c r="F14" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>155</v>
+      </c>
       <c r="H14" s="13" t="s">
         <v>128</v>
       </c>
@@ -2014,7 +2024,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B9" sqref="B9:C14"/>
     </sheetView>
@@ -2129,7 +2139,7 @@
         <v>91</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C9" s="19" t="s">
         <v>69</v>
@@ -2140,7 +2150,7 @@
         <v>91</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C10" s="19" t="s">
         <v>70</v>
@@ -2151,7 +2161,7 @@
         <v>91</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C11" s="19" t="s">
         <v>71</v>
@@ -2162,7 +2172,7 @@
         <v>91</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C12" s="19" t="s">
         <v>72</v>
@@ -2173,10 +2183,10 @@
         <v>91</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2184,10 +2194,10 @@
         <v>91</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2214,8 +2224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2238,10 +2248,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="10" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="C2" s="19" t="s">
         <v>78</v>

</xml_diff>